<commit_message>
Cluster sizing + Glow on click button + Paper listing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeel\Google Drive\master_project_and_literature_study\literature_study\visualization_DTs_ecosystems\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeel\Google Drive\master_project_and_literature_study\literature_study\visualization_DTs_ecosystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBE5B6E-511C-4D6D-A85D-B8A12DC5AC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FD1355-FBF0-4D71-9CF6-31B84A627ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="233">
   <si>
     <t>Type Paper</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>Stojanovic et al.</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>https://www.researchgate.net/publication/325737190_Towards_The_Generation_of_Digital_Twins_for_Facility_Management_Based_on_3D_Point_Clouds</t>
@@ -1218,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT926"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1226,7 @@
   <sheetData>
     <row r="1" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1418,7 +1415,7 @@
         <v>61</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BM1" s="7" t="s">
         <v>62</v>
@@ -2609,11 +2606,9 @@
       <c r="E13" s="9">
         <v>2018</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>75</v>
@@ -2705,11 +2700,9 @@
       <c r="E14" s="13">
         <v>2018</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="F14" s="12"/>
       <c r="G14" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12" t="s">
@@ -2793,19 +2786,19 @@
         <v>70</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="E15" s="9">
         <v>2022</v>
       </c>
       <c r="F15" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>75</v>
@@ -2889,19 +2882,19 @@
         <v>70</v>
       </c>
       <c r="C16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="E16" s="13">
         <v>2022</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>75</v>
@@ -2987,19 +2980,19 @@
         <v>70</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="E17" s="9">
         <v>2020</v>
       </c>
       <c r="F17" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>75</v>
@@ -3097,19 +3090,19 @@
         <v>70</v>
       </c>
       <c r="C18" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="E18" s="13">
         <v>2020</v>
       </c>
       <c r="F18" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>106</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>75</v>
@@ -3203,19 +3196,19 @@
         <v>70</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="E19" s="13">
         <v>2020</v>
       </c>
       <c r="F19" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>106</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12" t="s">
@@ -3305,19 +3298,19 @@
         <v>70</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="E20" s="9">
         <v>2022</v>
       </c>
       <c r="F20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>75</v>
@@ -3413,19 +3406,19 @@
         <v>70</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="E21" s="13">
         <v>2022</v>
       </c>
       <c r="F21" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>110</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>75</v>
@@ -3515,19 +3508,19 @@
         <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="E22" s="13">
         <v>2022</v>
       </c>
       <c r="F22" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>110</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12" t="s">
@@ -3621,19 +3614,19 @@
         <v>70</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="E23" s="9">
         <v>2020</v>
       </c>
       <c r="F23" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>75</v>
@@ -3725,19 +3718,19 @@
         <v>70</v>
       </c>
       <c r="C24" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="E24" s="13">
         <v>2020</v>
       </c>
       <c r="F24" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>114</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>75</v>
@@ -3831,19 +3824,19 @@
         <v>70</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="E25" s="9">
         <v>2020</v>
       </c>
       <c r="F25" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>75</v>
@@ -3945,19 +3938,19 @@
         <v>70</v>
       </c>
       <c r="C26" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>116</v>
       </c>
       <c r="E26" s="13">
         <v>2020</v>
       </c>
       <c r="F26" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>118</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>75</v>
@@ -4055,19 +4048,19 @@
         <v>70</v>
       </c>
       <c r="C27" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>116</v>
       </c>
       <c r="E27" s="13">
         <v>2020</v>
       </c>
       <c r="F27" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>118</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>75</v>
@@ -4161,19 +4154,17 @@
         <v>70</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="E28" s="9">
         <v>2021</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>95</v>
-      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>75</v>
@@ -4279,19 +4270,17 @@
         <v>70</v>
       </c>
       <c r="C29" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>120</v>
       </c>
       <c r="E29" s="13">
         <v>2021</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="F29" s="12"/>
       <c r="G29" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>75</v>
@@ -4389,19 +4378,17 @@
         <v>70</v>
       </c>
       <c r="C30" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>120</v>
       </c>
       <c r="E30" s="13">
         <v>2021</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>95</v>
-      </c>
+      <c r="F30" s="12"/>
       <c r="G30" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12" t="s">
@@ -4493,19 +4480,19 @@
         <v>70</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="E31" s="9">
         <v>2020</v>
       </c>
       <c r="F31" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>75</v>
@@ -4603,19 +4590,19 @@
         <v>70</v>
       </c>
       <c r="C32" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="E32" s="13">
         <v>2020</v>
       </c>
       <c r="F32" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>75</v>
@@ -4709,19 +4696,19 @@
         <v>70</v>
       </c>
       <c r="C33" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="E33" s="13">
         <v>2020</v>
       </c>
       <c r="F33" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12" t="s">
@@ -4815,19 +4802,19 @@
         <v>70</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="E34" s="9">
         <v>2022</v>
       </c>
       <c r="F34" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>129</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>75</v>
@@ -4925,19 +4912,19 @@
         <v>70</v>
       </c>
       <c r="C35" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="E35" s="13">
         <v>2022</v>
       </c>
       <c r="F35" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>129</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>75</v>
@@ -5029,19 +5016,19 @@
         <v>70</v>
       </c>
       <c r="C36" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>127</v>
       </c>
       <c r="E36" s="13">
         <v>2022</v>
       </c>
       <c r="F36" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>129</v>
       </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
@@ -5131,19 +5118,19 @@
         <v>70</v>
       </c>
       <c r="C37" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="E37" s="9">
         <v>2022</v>
       </c>
       <c r="F37" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" s="11" t="s">
         <v>132</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>133</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -5225,19 +5212,19 @@
         <v>70</v>
       </c>
       <c r="C38" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>131</v>
       </c>
       <c r="E38" s="13">
         <v>2022</v>
       </c>
       <c r="F38" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
@@ -5321,19 +5308,19 @@
         <v>70</v>
       </c>
       <c r="C39" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="E39" s="9">
         <v>2022</v>
       </c>
       <c r="F39" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>137</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -5421,19 +5408,19 @@
         <v>70</v>
       </c>
       <c r="C40" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>134</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="E40" s="13">
         <v>2022</v>
       </c>
       <c r="F40" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G40" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
@@ -5523,19 +5510,19 @@
         <v>70</v>
       </c>
       <c r="C41" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="E41" s="9">
         <v>2020</v>
       </c>
       <c r="F41" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>75</v>
@@ -5633,19 +5620,19 @@
         <v>70</v>
       </c>
       <c r="C42" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="E42" s="13">
         <v>2020</v>
       </c>
       <c r="F42" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>75</v>
@@ -5737,19 +5724,19 @@
         <v>70</v>
       </c>
       <c r="C43" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="E43" s="13">
         <v>2020</v>
       </c>
       <c r="F43" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G43" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>75</v>
@@ -5841,19 +5828,19 @@
         <v>70</v>
       </c>
       <c r="C44" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="E44" s="13">
         <v>2020</v>
       </c>
       <c r="F44" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G44" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="H44" s="12"/>
       <c r="I44" s="12" t="s">
@@ -5945,7 +5932,7 @@
         <v>70</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>79</v>
@@ -5954,10 +5941,10 @@
         <v>2020</v>
       </c>
       <c r="F45" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>75</v>
@@ -6049,7 +6036,7 @@
         <v>70</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>79</v>
@@ -6058,10 +6045,10 @@
         <v>2020</v>
       </c>
       <c r="F46" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G46" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>144</v>
       </c>
       <c r="H46" s="21" t="s">
         <v>75</v>
@@ -6155,19 +6142,19 @@
         <v>70</v>
       </c>
       <c r="C47" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="E47" s="9">
         <v>2022</v>
       </c>
       <c r="F47" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G47" s="11" t="s">
         <v>194</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>195</v>
       </c>
       <c r="H47" s="16" t="s">
         <v>75</v>
@@ -6257,19 +6244,19 @@
         <v>70</v>
       </c>
       <c r="C48" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D48" s="17" t="s">
         <v>192</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>193</v>
       </c>
       <c r="E48" s="18">
         <v>2022</v>
       </c>
       <c r="F48" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="G48" s="19" t="s">
         <v>194</v>
-      </c>
-      <c r="G48" s="19" t="s">
-        <v>195</v>
       </c>
       <c r="H48" s="20" t="s">
         <v>75</v>
@@ -6358,22 +6345,22 @@
         <v>1</v>
       </c>
       <c r="B49" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="E49" s="9">
         <v>2021</v>
       </c>
       <c r="F49" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>149</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>75</v>
@@ -6458,22 +6445,22 @@
     <row r="50" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="D50" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>147</v>
       </c>
       <c r="E50" s="13">
         <v>2021</v>
       </c>
       <c r="F50" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G50" s="15" t="s">
         <v>148</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>149</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>75</v>
@@ -6560,22 +6547,22 @@
         <v>2</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C51" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>151</v>
       </c>
       <c r="E51" s="9">
         <v>2022</v>
       </c>
       <c r="F51" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G51" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -6662,22 +6649,22 @@
     <row r="52" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="E52" s="13">
         <v>2022</v>
       </c>
       <c r="F52" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G52" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
@@ -6766,22 +6753,22 @@
         <v>3</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C53" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="E53" s="9">
         <v>2019</v>
       </c>
       <c r="F53" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G53" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>157</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6" t="s">
@@ -6862,22 +6849,22 @@
     <row r="54" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
       <c r="B54" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C54" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="12" t="s">
         <v>154</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>155</v>
       </c>
       <c r="E54" s="13">
         <v>2019</v>
       </c>
       <c r="F54" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G54" s="15" t="s">
         <v>156</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>157</v>
       </c>
       <c r="H54" s="12"/>
       <c r="I54" s="12" t="s">
@@ -6960,22 +6947,22 @@
         <v>4</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C55" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="E55" s="9">
         <v>2019</v>
       </c>
       <c r="F55" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G55" s="10" t="s">
         <v>160</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>161</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6" t="s">
@@ -7066,22 +7053,22 @@
     <row r="56" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
       <c r="B56" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C56" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>158</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>159</v>
       </c>
       <c r="E56" s="13">
         <v>2019</v>
       </c>
       <c r="F56" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G56" s="15" t="s">
         <v>160</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>161</v>
       </c>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
@@ -7174,22 +7161,22 @@
         <v>5</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C57" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="E57" s="9">
         <v>2018</v>
       </c>
       <c r="F57" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G57" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>165</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6" t="s">
@@ -7286,22 +7273,22 @@
     <row r="58" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
       <c r="B58" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C58" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>162</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>163</v>
       </c>
       <c r="E58" s="13">
         <v>2018</v>
       </c>
       <c r="F58" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G58" s="15" t="s">
         <v>164</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>165</v>
       </c>
       <c r="H58" s="12"/>
       <c r="I58" s="12" t="s">
@@ -7400,22 +7387,22 @@
         <v>6</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C59" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="E59" s="9">
         <v>2021</v>
       </c>
       <c r="F59" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G59" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>169</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>75</v>
@@ -7504,22 +7491,22 @@
     <row r="60" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12"/>
       <c r="B60" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C60" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>167</v>
       </c>
       <c r="E60" s="13">
         <v>2021</v>
       </c>
       <c r="F60" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>169</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>75</v>
@@ -7610,22 +7597,22 @@
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C61" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>171</v>
       </c>
       <c r="E61" s="9">
         <v>2022</v>
       </c>
       <c r="F61" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="G61" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="G61" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -7708,22 +7695,22 @@
     <row r="62" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
       <c r="B62" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>170</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>171</v>
       </c>
       <c r="E62" s="13">
         <v>2022</v>
       </c>
       <c r="F62" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G62" s="15" t="s">
         <v>172</v>
-      </c>
-      <c r="G62" s="15" t="s">
-        <v>173</v>
       </c>
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
@@ -7808,22 +7795,22 @@
         <v>8</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C63" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="E63" s="9">
         <v>2020</v>
       </c>
       <c r="F63" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>177</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6" t="s">
@@ -7914,22 +7901,22 @@
     <row r="64" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="B64" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>174</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>175</v>
       </c>
       <c r="E64" s="13">
         <v>2020</v>
       </c>
       <c r="F64" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G64" s="15" t="s">
         <v>176</v>
-      </c>
-      <c r="G64" s="15" t="s">
-        <v>177</v>
       </c>
       <c r="H64" s="12"/>
       <c r="I64" s="12" t="s">
@@ -8022,22 +8009,22 @@
         <v>9</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C65" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="E65" s="9">
         <v>2021</v>
       </c>
       <c r="F65" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G65" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="G65" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6" t="s">
@@ -8122,22 +8109,22 @@
     <row r="66" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C66" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>178</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>179</v>
       </c>
       <c r="E66" s="13">
         <v>2021</v>
       </c>
       <c r="F66" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="G66" s="15" t="s">
         <v>180</v>
-      </c>
-      <c r="G66" s="15" t="s">
-        <v>181</v>
       </c>
       <c r="H66" s="12"/>
       <c r="I66" s="12" t="s">
@@ -8224,22 +8211,22 @@
         <v>10</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C67" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="E67" s="9">
         <v>2021</v>
       </c>
       <c r="F67" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G67" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>185</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>75</v>
@@ -8326,22 +8313,22 @@
     <row r="68" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C68" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D68" s="12" t="s">
         <v>182</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>183</v>
       </c>
       <c r="E68" s="13">
         <v>2021</v>
       </c>
       <c r="F68" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G68" s="15" t="s">
         <v>184</v>
-      </c>
-      <c r="G68" s="15" t="s">
-        <v>185</v>
       </c>
       <c r="H68" s="12" t="s">
         <v>75</v>
@@ -8424,22 +8411,22 @@
     <row r="69" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C69" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" s="12" t="s">
         <v>182</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>183</v>
       </c>
       <c r="E69" s="13">
         <v>2021</v>
       </c>
       <c r="F69" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G69" s="15" t="s">
         <v>184</v>
-      </c>
-      <c r="G69" s="15" t="s">
-        <v>185</v>
       </c>
       <c r="H69" s="12"/>
       <c r="I69" s="12" t="s">
@@ -8522,22 +8509,22 @@
         <v>11</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C70" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="E70" s="9">
         <v>2019</v>
       </c>
       <c r="F70" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="G70" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
@@ -8622,22 +8609,22 @@
     <row r="71" spans="1:72" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C71" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D71" s="12" t="s">
         <v>186</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>187</v>
       </c>
       <c r="E71" s="13">
         <v>2019</v>
       </c>
       <c r="F71" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G71" s="15" t="s">
         <v>188</v>
-      </c>
-      <c r="G71" s="15" t="s">
-        <v>189</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
@@ -72082,7 +72069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99F4AA7-9738-4229-9559-79AF3E628185}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Z35" sqref="Z35"/>
     </sheetView>
@@ -72091,61 +72078,61 @@
   <sheetData>
     <row r="1" spans="1:19" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>198</v>
-      </c>
       <c r="D1" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="I1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="N1" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="O1" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="P1" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="R1" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="S1" s="22" t="s">
         <v>226</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -72153,7 +72140,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -72161,7 +72148,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -72169,7 +72156,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -72177,7 +72164,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -72185,7 +72172,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -72193,7 +72180,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -72201,7 +72188,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -72209,7 +72196,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -72217,7 +72204,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -72225,7 +72212,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -72233,7 +72220,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -72241,7 +72228,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -72260,10 +72247,10 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C15" t="s">
         <v>211</v>
-      </c>
-      <c r="C15" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -72271,7 +72258,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -72290,7 +72277,7 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
@@ -72301,7 +72288,7 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -72312,7 +72299,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
@@ -72323,7 +72310,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -72334,7 +72321,7 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
@@ -72345,7 +72332,7 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
@@ -72356,7 +72343,7 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -72367,7 +72354,7 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -72378,7 +72365,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
@@ -72389,7 +72376,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C27" t="s">
         <v>31</v>
@@ -72400,7 +72387,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C28" t="s">
         <v>32</v>
@@ -72411,7 +72398,7 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
@@ -72422,7 +72409,7 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -72433,7 +72420,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
@@ -72444,7 +72431,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>36</v>
@@ -72455,7 +72442,7 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -72466,7 +72453,7 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
@@ -72477,7 +72464,7 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C35" t="s">
         <v>39</v>
@@ -72488,7 +72475,7 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C36" t="s">
         <v>40</v>
@@ -72507,7 +72494,7 @@
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C38" t="s">
         <v>42</v>
@@ -72526,7 +72513,7 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -72561,7 +72548,7 @@
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C44" t="s">
         <v>48</v>
@@ -72580,7 +72567,7 @@
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" t="s">
         <v>50</v>
@@ -72591,7 +72578,7 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C47" t="s">
         <v>51</v>
@@ -72602,7 +72589,7 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C48" t="s">
         <v>52</v>
@@ -72613,7 +72600,7 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C49" t="s">
         <v>53</v>
@@ -72624,7 +72611,7 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C50" t="s">
         <v>54</v>
@@ -72659,7 +72646,7 @@
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C54" t="s">
         <v>58</v>
@@ -72670,7 +72657,7 @@
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C55" t="s">
         <v>59</v>
@@ -72681,7 +72668,7 @@
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C56" t="s">
         <v>60</v>
@@ -72697,10 +72684,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -72732,7 +72719,7 @@
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C62" t="s">
         <v>65</v>
@@ -72743,7 +72730,7 @@
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C63" t="s">
         <v>66</v>
@@ -72754,7 +72741,7 @@
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C64" t="s">
         <v>67</v>
@@ -72765,7 +72752,7 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C65" t="s">
         <v>68</v>
@@ -72776,7 +72763,7 @@
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C66" t="s">
         <v>69</v>

</xml_diff>